<commit_message>
put notes in Straight.xlsx
</commit_message>
<xml_diff>
--- a/data/Straight.xlsx
+++ b/data/Straight.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmargani/sandbox/robotics/EV3Python2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046C242-44F4-7C45-93FB-35DCC3AF8C3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
+    <workbookView xWindow="35840" yWindow="960" windowWidth="34040" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>A-C: gain = 1.4</t>
   </si>
@@ -34,11 +35,47 @@
   <si>
     <t>A = no disturbance</t>
   </si>
+  <si>
+    <t>x axis - sort of time</t>
+  </si>
+  <si>
+    <t>y axis - correction</t>
+  </si>
+  <si>
+    <t>Run 1 - robot goes pretty straight when not disturbed!  Gyro sensor angles never go past 1 or -1, and most of the time it's at zero!</t>
+  </si>
+  <si>
+    <t>our robot got disturbed at row number 32, and got pushed all the way to an angle of -47/1.4 = -33.  Wow.  But it eventually straightens out by row number 100, and has only a small overshoot.</t>
+  </si>
+  <si>
+    <t>We smacked the robot at row number 36, but not hard enough!  So not a great experiment.  Near the end it hovers around 1 degree instead of zero.  We don't know why.</t>
+  </si>
+  <si>
+    <t>at row number 40, we hit the robot to -90/1.4 = -67 degrees!  Twice as hard as Run 2!</t>
+  </si>
+  <si>
+    <t>With a gain of 5.0, we go from -67 to 0 degrees in about 20.</t>
+  </si>
+  <si>
+    <t>we hit the robot at 32, and got zero by 95, that's 95 - 32 = 63 row numbers.</t>
+  </si>
+  <si>
+    <t>conclusion: the larger gain means we recover from the disturbance much faster.  Hardly any overshoot!</t>
+  </si>
+  <si>
+    <t>after the disturbanc remains pretty straight.</t>
+  </si>
+  <si>
+    <t>Conclusion: run 4 is like run 5.</t>
+  </si>
+  <si>
+    <t>Maybe next time, increase the gain till we see ocsillation!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,13 +178,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 1</a:t>
+              <a:t> 1 - A, gain = 1.4, no distrubance </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1449,13 +1485,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2</a:t>
+              <a:t> 2 - B, gain = 1.4</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2116,7 +2151,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Run 3</a:t>
+              <a:t>Run 3 - C, gain = 1.4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3417,13 +3452,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 4</a:t>
+              <a:t> 4 - D, gain = 5.0</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4769,13 +4802,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 5</a:t>
+              <a:t> 5 - E, gain = 5.0</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8835,20 +8867,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>321</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>288925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>335</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8878,7 +8916,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8895,20 +8939,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>479425</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>60325</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8938,7 +8988,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8968,7 +9024,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9248,19 +9310,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J409"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U409"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -9280,7 +9342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -9297,7 +9359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -9310,8 +9372,11 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1.4</v>
       </c>
@@ -9324,8 +9389,11 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.4</v>
       </c>
@@ -9339,7 +9407,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1.4</v>
       </c>
@@ -9353,7 +9421,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1.4</v>
       </c>
@@ -9367,7 +9435,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.4</v>
       </c>
@@ -9381,7 +9449,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -9395,7 +9463,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.4</v>
       </c>
@@ -9409,7 +9477,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -9423,7 +9491,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -9437,7 +9505,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -9451,7 +9519,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -9465,7 +9533,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1.4</v>
       </c>
@@ -9479,7 +9547,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1.4</v>
       </c>
@@ -9493,7 +9561,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1.4</v>
       </c>
@@ -9507,7 +9575,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1.4</v>
       </c>
@@ -9521,7 +9589,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1.4</v>
       </c>
@@ -9535,7 +9603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1.4</v>
       </c>
@@ -9549,7 +9617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1.4</v>
       </c>
@@ -9562,8 +9630,11 @@
       <c r="E21" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1.4</v>
       </c>
@@ -9577,7 +9648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -9591,7 +9662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -9605,7 +9676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -9618,8 +9689,11 @@
       <c r="E25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>-1.4</v>
       </c>
@@ -9632,8 +9706,11 @@
       <c r="E26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -9646,8 +9723,11 @@
       <c r="E27" s="1">
         <v>-5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -9660,8 +9740,11 @@
       <c r="E28" s="1">
         <v>-5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -9675,7 +9758,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -9689,7 +9772,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -9703,7 +9786,7 @@
         <v>-75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -9717,7 +9800,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -9731,7 +9814,7 @@
         <v>-115</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -9745,7 +9828,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -9759,7 +9842,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -9773,7 +9856,7 @@
         <v>-85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -9787,7 +9870,7 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -9801,7 +9884,7 @@
         <v>-55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>0</v>
       </c>
@@ -9815,7 +9898,7 @@
         <v>-45</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -9829,7 +9912,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>0</v>
       </c>
@@ -9843,7 +9926,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>0</v>
       </c>
@@ -9857,7 +9940,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>0</v>
       </c>
@@ -9871,7 +9954,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>0</v>
       </c>
@@ -9885,7 +9968,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>0</v>
       </c>
@@ -9899,7 +9982,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>0</v>
       </c>
@@ -9913,7 +9996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>0</v>
       </c>
@@ -9927,7 +10010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0</v>
       </c>
@@ -9941,7 +10024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>0</v>
       </c>
@@ -9955,7 +10038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>0</v>
       </c>
@@ -9969,7 +10052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>0</v>
       </c>
@@ -9982,8 +10065,11 @@
       <c r="E51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="U51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>0</v>
       </c>
@@ -9996,8 +10082,11 @@
       <c r="E52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>0</v>
       </c>
@@ -10011,7 +10100,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>0</v>
       </c>
@@ -10025,7 +10114,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>0</v>
       </c>
@@ -10039,7 +10128,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>0</v>
       </c>
@@ -10053,7 +10142,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>0</v>
       </c>
@@ -10066,8 +10155,11 @@
       <c r="E57" s="1">
         <v>-10</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>0</v>
       </c>
@@ -10081,7 +10173,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>0</v>
       </c>
@@ -10095,7 +10187,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>0</v>
       </c>
@@ -10109,7 +10201,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>0</v>
       </c>
@@ -10123,7 +10215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>0</v>
       </c>
@@ -10137,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>0</v>
       </c>
@@ -10151,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>0</v>
       </c>
@@ -10165,7 +10257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>1.4</v>
       </c>
@@ -10179,7 +10271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>1.4</v>
       </c>
@@ -10193,7 +10285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>1.4</v>
       </c>
@@ -10207,7 +10299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>1.4</v>
       </c>
@@ -10221,7 +10313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>1.4</v>
       </c>
@@ -10235,7 +10327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>1.4</v>
       </c>
@@ -10252,7 +10344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>1.4</v>
       </c>
@@ -10269,7 +10361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>0</v>
       </c>
@@ -10286,7 +10378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>0</v>
       </c>
@@ -10303,7 +10395,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>0</v>
       </c>
@@ -10320,7 +10412,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>0</v>
       </c>
@@ -10337,7 +10429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>0</v>
       </c>
@@ -10354,7 +10446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>0</v>
       </c>
@@ -10371,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>0</v>
       </c>
@@ -10388,7 +10480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>0</v>
       </c>
@@ -10405,7 +10497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>0</v>
       </c>
@@ -10422,7 +10514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>0</v>
       </c>
@@ -10439,7 +10531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>1.4</v>
       </c>
@@ -10456,7 +10548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>1.4</v>
       </c>
@@ -10473,7 +10565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -10490,7 +10582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>0</v>
       </c>
@@ -10507,7 +10599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>0</v>
       </c>
@@ -10524,7 +10616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>0</v>
       </c>
@@ -10541,7 +10633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>0</v>
       </c>
@@ -10558,7 +10650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>0</v>
       </c>
@@ -10575,7 +10667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>0</v>
       </c>
@@ -10592,7 +10684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>0</v>
       </c>
@@ -10608,8 +10700,11 @@
       <c r="E91" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>0</v>
       </c>
@@ -10625,8 +10720,11 @@
       <c r="E92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>0</v>
       </c>
@@ -10643,7 +10741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>0</v>
       </c>
@@ -10660,7 +10758,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>-1.4</v>
       </c>
@@ -10677,7 +10775,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>-1.4</v>
       </c>
@@ -10694,7 +10792,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>-1.4</v>
       </c>
@@ -10711,7 +10809,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>-1.4</v>
       </c>
@@ -10728,7 +10826,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>-1.4</v>
       </c>
@@ -10745,7 +10843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>-1.4</v>
       </c>
@@ -10762,7 +10860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>-1.4</v>
       </c>
@@ -10779,7 +10877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>-1.4</v>
       </c>
@@ -10796,7 +10894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>-1.4</v>
       </c>
@@ -10813,7 +10911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>0</v>
       </c>
@@ -10830,7 +10928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>0</v>
       </c>
@@ -10847,7 +10945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>0</v>
       </c>
@@ -10864,7 +10962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>0</v>
       </c>
@@ -10881,7 +10979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>0</v>
       </c>
@@ -10898,7 +10996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>0</v>
       </c>
@@ -10915,7 +11013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>0</v>
       </c>
@@ -10932,7 +11030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>0</v>
       </c>
@@ -10949,7 +11047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>0</v>
       </c>
@@ -10966,7 +11064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>0</v>
       </c>
@@ -10983,7 +11081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>0</v>
       </c>
@@ -11000,7 +11098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>0</v>
       </c>
@@ -11017,7 +11115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>0</v>
       </c>
@@ -11034,7 +11132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>0</v>
       </c>
@@ -11051,7 +11149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>0</v>
       </c>
@@ -11068,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>0</v>
       </c>
@@ -11085,7 +11183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>0</v>
       </c>
@@ -11102,7 +11200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>0</v>
       </c>
@@ -11119,7 +11217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>0</v>
       </c>
@@ -11136,7 +11234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>0</v>
       </c>
@@ -11153,7 +11251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>0</v>
       </c>
@@ -11170,7 +11268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>1.4</v>
       </c>
@@ -11187,7 +11285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>1.4</v>
       </c>
@@ -11204,7 +11302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>1.4</v>
       </c>
@@ -11221,7 +11319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>1.4</v>
       </c>
@@ -11238,7 +11336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>1.4</v>
       </c>
@@ -11255,7 +11353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>0</v>
       </c>
@@ -11272,7 +11370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>0</v>
       </c>
@@ -11289,7 +11387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>0</v>
       </c>
@@ -11306,7 +11404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>0</v>
       </c>
@@ -11320,7 +11418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>0</v>
       </c>
@@ -11334,7 +11432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>0</v>
       </c>
@@ -11348,7 +11446,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>0</v>
       </c>
@@ -11362,7 +11460,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>0</v>
       </c>
@@ -11376,7 +11474,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>0</v>
       </c>
@@ -11390,7 +11488,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>0</v>
       </c>
@@ -11404,7 +11502,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>0</v>
       </c>
@@ -11418,7 +11516,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>0</v>
       </c>
@@ -11432,7 +11530,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>0</v>
       </c>
@@ -11446,7 +11544,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>0</v>
       </c>
@@ -11460,7 +11558,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>0</v>
       </c>
@@ -11474,7 +11572,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>0</v>
       </c>
@@ -11488,7 +11586,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>0</v>
       </c>
@@ -11502,7 +11600,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>0</v>
       </c>
@@ -11516,7 +11614,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>0</v>
       </c>
@@ -11530,7 +11628,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>0</v>
       </c>
@@ -11544,7 +11642,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>0</v>
       </c>
@@ -11558,7 +11656,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>0</v>
       </c>
@@ -11572,7 +11670,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>0</v>
       </c>
@@ -11586,7 +11684,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>0</v>
       </c>
@@ -11600,7 +11698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>0</v>
       </c>
@@ -11614,7 +11712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>0</v>
       </c>
@@ -11628,7 +11726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>0</v>
       </c>
@@ -11642,7 +11740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>1.4</v>
       </c>
@@ -11656,7 +11754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>1.4</v>
       </c>
@@ -11670,7 +11768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>0</v>
       </c>
@@ -11684,7 +11782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>0</v>
       </c>
@@ -11698,7 +11796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>0</v>
       </c>
@@ -11712,7 +11810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>0</v>
       </c>
@@ -11726,7 +11824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>0</v>
       </c>
@@ -11740,7 +11838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>0</v>
       </c>
@@ -11754,7 +11852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>0</v>
       </c>
@@ -11768,7 +11866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>0</v>
       </c>
@@ -11782,7 +11880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>0</v>
       </c>
@@ -11796,7 +11894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>0</v>
       </c>
@@ -11810,7 +11908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>0</v>
       </c>
@@ -11824,7 +11922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>0</v>
       </c>
@@ -11838,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>0</v>
       </c>
@@ -11852,7 +11950,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>0</v>
       </c>
@@ -11866,7 +11964,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>0</v>
       </c>
@@ -11880,7 +11978,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>0</v>
       </c>
@@ -11894,7 +11992,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>0</v>
       </c>
@@ -11908,7 +12006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>0</v>
       </c>
@@ -11922,7 +12020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>0</v>
       </c>
@@ -11936,7 +12034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>0</v>
       </c>
@@ -11950,7 +12048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>0</v>
       </c>
@@ -11964,7 +12062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>0</v>
       </c>
@@ -11978,7 +12076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>0</v>
       </c>
@@ -11992,7 +12090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>0</v>
       </c>
@@ -12006,7 +12104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>0</v>
       </c>
@@ -12020,7 +12118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>0</v>
       </c>
@@ -12034,7 +12132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>0</v>
       </c>
@@ -12048,7 +12146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>1.4</v>
       </c>
@@ -12062,7 +12160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>1.4</v>
       </c>
@@ -12076,7 +12174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>0</v>
       </c>
@@ -12090,7 +12188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>0</v>
       </c>
@@ -12104,7 +12202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>0</v>
       </c>
@@ -12118,7 +12216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>0</v>
       </c>
@@ -12132,7 +12230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>0</v>
       </c>
@@ -12146,7 +12244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>1.4</v>
       </c>
@@ -12160,7 +12258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>1.4</v>
       </c>
@@ -12174,7 +12272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>0</v>
       </c>
@@ -12188,7 +12286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>1.4</v>
       </c>
@@ -12202,7 +12300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>0</v>
       </c>
@@ -12216,7 +12314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>0</v>
       </c>
@@ -12230,7 +12328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>0</v>
       </c>
@@ -12244,7 +12342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>0</v>
       </c>
@@ -12258,7 +12356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>0</v>
       </c>
@@ -12272,7 +12370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>0</v>
       </c>
@@ -12286,7 +12384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>0</v>
       </c>
@@ -12300,7 +12398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>0</v>
       </c>
@@ -12314,7 +12412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>0</v>
       </c>
@@ -12328,7 +12426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>0</v>
       </c>
@@ -12342,7 +12440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>0</v>
       </c>
@@ -12356,7 +12454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>0</v>
       </c>
@@ -12370,7 +12468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>0</v>
       </c>
@@ -12384,7 +12482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>0</v>
       </c>
@@ -12398,7 +12496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>0</v>
       </c>
@@ -12412,7 +12510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>0</v>
       </c>
@@ -12426,7 +12524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>0</v>
       </c>
@@ -12440,7 +12538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>0</v>
       </c>
@@ -12454,7 +12552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>0</v>
       </c>
@@ -12468,7 +12566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>0</v>
       </c>
@@ -12482,7 +12580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>0</v>
       </c>
@@ -12496,7 +12594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>0</v>
       </c>
@@ -12510,7 +12608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>0</v>
       </c>
@@ -12524,7 +12622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>0</v>
       </c>
@@ -12538,7 +12636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>0</v>
       </c>
@@ -12552,7 +12650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>0</v>
       </c>
@@ -12566,7 +12664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>0</v>
       </c>
@@ -12580,7 +12678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>0</v>
       </c>
@@ -12594,7 +12692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>0</v>
       </c>
@@ -12608,7 +12706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>0</v>
       </c>
@@ -12622,7 +12720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>0</v>
       </c>
@@ -12636,7 +12734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>0</v>
       </c>
@@ -12650,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>0</v>
       </c>
@@ -12664,7 +12762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>0</v>
       </c>
@@ -12678,7 +12776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>0</v>
       </c>
@@ -12692,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>0</v>
       </c>
@@ -12706,7 +12804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>0</v>
       </c>
@@ -12720,7 +12818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>0</v>
       </c>
@@ -12734,7 +12832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>0</v>
       </c>
@@ -12748,7 +12846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>0</v>
       </c>
@@ -12762,7 +12860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>0</v>
       </c>
@@ -12776,7 +12874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>0</v>
       </c>
@@ -12790,7 +12888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>0</v>
       </c>
@@ -12804,7 +12902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>0</v>
       </c>
@@ -12818,7 +12916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>0</v>
       </c>
@@ -12832,7 +12930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>0</v>
       </c>
@@ -12846,7 +12944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>0</v>
       </c>
@@ -12860,7 +12958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>0</v>
       </c>
@@ -12874,7 +12972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>0</v>
       </c>
@@ -12888,7 +12986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>0</v>
       </c>
@@ -12902,7 +13000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>0</v>
       </c>
@@ -12916,7 +13014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>0</v>
       </c>
@@ -12930,7 +13028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>0</v>
       </c>
@@ -12944,7 +13042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>0</v>
       </c>
@@ -12958,7 +13056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>0</v>
       </c>
@@ -12972,7 +13070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>0</v>
       </c>
@@ -12986,7 +13084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>0</v>
       </c>
@@ -13000,7 +13098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>0</v>
       </c>
@@ -13014,7 +13112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>0</v>
       </c>
@@ -13028,7 +13126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>0</v>
       </c>
@@ -13042,7 +13140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>0</v>
       </c>
@@ -13056,7 +13154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>0</v>
       </c>
@@ -13070,7 +13168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>0</v>
       </c>
@@ -13084,7 +13182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>0</v>
       </c>
@@ -13098,7 +13196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>0</v>
       </c>
@@ -13112,7 +13210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>0</v>
       </c>
@@ -13126,7 +13224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>0</v>
       </c>
@@ -13140,7 +13238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>0</v>
       </c>
@@ -13154,7 +13252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>0</v>
       </c>
@@ -13168,7 +13266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>0</v>
       </c>
@@ -13182,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>0</v>
       </c>
@@ -13196,7 +13294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>0</v>
       </c>
@@ -13210,7 +13308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>0</v>
       </c>
@@ -13224,7 +13322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>0</v>
       </c>
@@ -13238,7 +13336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>0</v>
       </c>
@@ -13252,7 +13350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>0</v>
       </c>
@@ -13266,7 +13364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>0</v>
       </c>
@@ -13280,7 +13378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>0</v>
       </c>
@@ -13294,7 +13392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>0</v>
       </c>
@@ -13308,7 +13406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>0</v>
       </c>
@@ -13322,7 +13420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>0</v>
       </c>
@@ -13336,7 +13434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>0</v>
       </c>
@@ -13350,7 +13448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>0</v>
       </c>
@@ -13364,7 +13462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>0</v>
       </c>
@@ -13378,7 +13476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>0</v>
       </c>
@@ -13392,7 +13490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>0</v>
       </c>
@@ -13406,7 +13504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>0</v>
       </c>
@@ -13420,7 +13518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>0</v>
       </c>
@@ -13434,7 +13532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>0</v>
       </c>
@@ -13448,7 +13546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>0</v>
       </c>
@@ -13462,7 +13560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>0</v>
       </c>
@@ -13476,7 +13574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>0</v>
       </c>
@@ -13490,7 +13588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>0</v>
       </c>
@@ -13504,7 +13602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>0</v>
       </c>
@@ -13518,7 +13616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>0</v>
       </c>
@@ -13532,7 +13630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>0</v>
       </c>
@@ -13546,7 +13644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>0</v>
       </c>
@@ -13560,7 +13658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>0</v>
       </c>
@@ -13574,7 +13672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>0</v>
       </c>
@@ -13588,7 +13686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>0</v>
       </c>
@@ -13602,7 +13700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>0</v>
       </c>
@@ -13616,7 +13714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>0</v>
       </c>
@@ -13630,7 +13728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>0</v>
       </c>
@@ -13644,7 +13742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>0</v>
       </c>
@@ -13658,7 +13756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>0</v>
       </c>
@@ -13672,7 +13770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>0</v>
       </c>
@@ -13686,7 +13784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>0</v>
       </c>
@@ -13700,7 +13798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>0</v>
       </c>
@@ -13714,7 +13812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>0</v>
       </c>
@@ -13728,7 +13826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>0</v>
       </c>
@@ -13742,7 +13840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>0</v>
       </c>
@@ -13756,7 +13854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>0</v>
       </c>
@@ -13770,7 +13868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>0</v>
       </c>
@@ -13784,7 +13882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>0</v>
       </c>
@@ -13798,7 +13896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>0</v>
       </c>
@@ -13812,7 +13910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>0</v>
       </c>
@@ -13826,7 +13924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>0</v>
       </c>
@@ -13840,7 +13938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>-1.4</v>
       </c>
@@ -13854,7 +13952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>-1.4</v>
       </c>
@@ -13868,7 +13966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>-1.4</v>
       </c>
@@ -13882,7 +13980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>-1.4</v>
       </c>
@@ -13896,7 +13994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>-1.4</v>
       </c>
@@ -13910,7 +14008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>-1.4</v>
       </c>
@@ -13924,7 +14022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>-1.4</v>
       </c>
@@ -13938,7 +14036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>-1.4</v>
       </c>
@@ -13952,7 +14050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>-1.4</v>
       </c>
@@ -13966,7 +14064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>-1.4</v>
       </c>
@@ -13980,7 +14078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>-1.4</v>
       </c>
@@ -13994,7 +14092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>-1.4</v>
       </c>
@@ -14008,7 +14106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>-1.4</v>
       </c>
@@ -14022,7 +14120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>-1.4</v>
       </c>
@@ -14036,7 +14134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>-1.4</v>
       </c>
@@ -14050,7 +14148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>-1.4</v>
       </c>
@@ -14064,7 +14162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>-1.4</v>
       </c>
@@ -14078,7 +14176,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>-1.4</v>
       </c>
@@ -14092,7 +14190,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>0</v>
       </c>
@@ -14106,7 +14204,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>0</v>
       </c>
@@ -14120,7 +14218,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>0</v>
       </c>
@@ -14134,7 +14232,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>0</v>
       </c>
@@ -14148,7 +14246,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>0</v>
       </c>
@@ -14162,7 +14260,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>0</v>
       </c>
@@ -14176,7 +14274,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>0</v>
       </c>
@@ -14190,7 +14288,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>0</v>
       </c>
@@ -14204,7 +14302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>0</v>
       </c>
@@ -14218,7 +14316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C341" s="1">
         <v>0</v>
       </c>
@@ -14229,7 +14327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C342" s="1">
         <v>0</v>
       </c>
@@ -14240,7 +14338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C343" s="1">
         <v>0</v>
       </c>
@@ -14251,7 +14349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C344" s="1">
         <v>0</v>
       </c>
@@ -14262,7 +14360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C345" s="1">
         <v>0</v>
       </c>
@@ -14273,7 +14371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C346" s="1">
         <v>0</v>
       </c>
@@ -14284,7 +14382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C347" s="1">
         <v>0</v>
       </c>
@@ -14295,7 +14393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C348" s="1">
         <v>1.4</v>
       </c>
@@ -14306,7 +14404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C349" s="1">
         <v>1.4</v>
       </c>
@@ -14317,7 +14415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C350" s="1">
         <v>1.4</v>
       </c>
@@ -14328,7 +14426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C351" s="1">
         <v>1.4</v>
       </c>
@@ -14339,7 +14437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C352" s="1">
         <v>1.4</v>
       </c>
@@ -14350,7 +14448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C353" s="1">
         <v>1.4</v>
       </c>
@@ -14361,7 +14459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C354" s="1">
         <v>1.4</v>
       </c>
@@ -14369,7 +14467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C355" s="1">
         <v>1.4</v>
       </c>
@@ -14377,7 +14475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C356" s="1">
         <v>1.4</v>
       </c>
@@ -14385,7 +14483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="357" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C357" s="1">
         <v>1.4</v>
       </c>
@@ -14393,7 +14491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="358" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C358" s="1">
         <v>1.4</v>
       </c>
@@ -14401,7 +14499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="359" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C359" s="1">
         <v>1.4</v>
       </c>
@@ -14409,252 +14507,252 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C360" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="361" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C361" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="362" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C362" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="363" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C363" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="364" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C364" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="365" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C365" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="366" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C366" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="367" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C367" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="368" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C368" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="369" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C369" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="370" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C370" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C371" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="372" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C372" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="373" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C373" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="374" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C374" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="375" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C375" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="376" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C376" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="377" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C377" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="378" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C378" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="379" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C379" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="380" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C380" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="381" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C381" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="382" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C382" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="383" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C383" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="384" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C384" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="385" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C385" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="386" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C386" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="387" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C387" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="388" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C388" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="389" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C389" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="390" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C390" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="391" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C391" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="392" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C392" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="393" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C393" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="394" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C394" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="395" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C395" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="396" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C396" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="397" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C397" s="1">
         <v>1.4</v>
       </c>
     </row>
-    <row r="398" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C398" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="399" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C399" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="400" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C400" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="401" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C401" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="402" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C402" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="403" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C403" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="404" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C404" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="405" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C405" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="406" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C406" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="407" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C407" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="408" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C408" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="409" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C409" s="1">
         <v>2.8</v>
       </c>

</xml_diff>